<commit_message>
update excel mhs dan dosen
</commit_message>
<xml_diff>
--- a/public/template_dosen.xlsx
+++ b/public/template_dosen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\PBL4_Sem4\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A90360E1-2E04-4E89-9E46-FF9E8798D42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FC3A60-4809-4335-A836-B231EF6F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D6DA15E-DDB3-4EFE-A360-522A40B24874}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="209">
   <si>
     <t>username</t>
   </si>
@@ -58,13 +58,616 @@
   </si>
   <si>
     <t>dosen2@gmail.com</t>
+  </si>
+  <si>
+    <t>dosen101</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>Dosen 101</t>
+  </si>
+  <si>
+    <t>dosen101@example.com</t>
+  </si>
+  <si>
+    <t>3975120270055</t>
+  </si>
+  <si>
+    <t>dosen102</t>
+  </si>
+  <si>
+    <t>Dosen 102</t>
+  </si>
+  <si>
+    <t>dosen102@example.com</t>
+  </si>
+  <si>
+    <t>0991078851835</t>
+  </si>
+  <si>
+    <t>dosen103</t>
+  </si>
+  <si>
+    <t>Dosen 103</t>
+  </si>
+  <si>
+    <t>dosen103@example.com</t>
+  </si>
+  <si>
+    <t>5538439004811</t>
+  </si>
+  <si>
+    <t>dosen104</t>
+  </si>
+  <si>
+    <t>Dosen 104</t>
+  </si>
+  <si>
+    <t>dosen104@example.com</t>
+  </si>
+  <si>
+    <t>5678431614668</t>
+  </si>
+  <si>
+    <t>dosen105</t>
+  </si>
+  <si>
+    <t>Dosen 105</t>
+  </si>
+  <si>
+    <t>dosen105@example.com</t>
+  </si>
+  <si>
+    <t>3048052825041</t>
+  </si>
+  <si>
+    <t>dosen106</t>
+  </si>
+  <si>
+    <t>Dosen 106</t>
+  </si>
+  <si>
+    <t>dosen106@example.com</t>
+  </si>
+  <si>
+    <t>0027897990903</t>
+  </si>
+  <si>
+    <t>dosen107</t>
+  </si>
+  <si>
+    <t>Dosen 107</t>
+  </si>
+  <si>
+    <t>dosen107@example.com</t>
+  </si>
+  <si>
+    <t>1171124852836</t>
+  </si>
+  <si>
+    <t>dosen108</t>
+  </si>
+  <si>
+    <t>Dosen 108</t>
+  </si>
+  <si>
+    <t>dosen108@example.com</t>
+  </si>
+  <si>
+    <t>3155414391235</t>
+  </si>
+  <si>
+    <t>dosen109</t>
+  </si>
+  <si>
+    <t>Dosen 109</t>
+  </si>
+  <si>
+    <t>dosen109@example.com</t>
+  </si>
+  <si>
+    <t>3283242900379</t>
+  </si>
+  <si>
+    <t>dosen110</t>
+  </si>
+  <si>
+    <t>Dosen 110</t>
+  </si>
+  <si>
+    <t>dosen110@example.com</t>
+  </si>
+  <si>
+    <t>2701104474890</t>
+  </si>
+  <si>
+    <t>dosen111</t>
+  </si>
+  <si>
+    <t>Dosen 111</t>
+  </si>
+  <si>
+    <t>dosen111@example.com</t>
+  </si>
+  <si>
+    <t>3616771829246</t>
+  </si>
+  <si>
+    <t>dosen112</t>
+  </si>
+  <si>
+    <t>Dosen 112</t>
+  </si>
+  <si>
+    <t>dosen112@example.com</t>
+  </si>
+  <si>
+    <t>2669629346796</t>
+  </si>
+  <si>
+    <t>dosen113</t>
+  </si>
+  <si>
+    <t>Dosen 113</t>
+  </si>
+  <si>
+    <t>dosen113@example.com</t>
+  </si>
+  <si>
+    <t>8332749022913</t>
+  </si>
+  <si>
+    <t>dosen114</t>
+  </si>
+  <si>
+    <t>Dosen 114</t>
+  </si>
+  <si>
+    <t>dosen114@example.com</t>
+  </si>
+  <si>
+    <t>4122970652007</t>
+  </si>
+  <si>
+    <t>dosen115</t>
+  </si>
+  <si>
+    <t>Dosen 115</t>
+  </si>
+  <si>
+    <t>dosen115@example.com</t>
+  </si>
+  <si>
+    <t>4306261782980</t>
+  </si>
+  <si>
+    <t>dosen116</t>
+  </si>
+  <si>
+    <t>Dosen 116</t>
+  </si>
+  <si>
+    <t>dosen116@example.com</t>
+  </si>
+  <si>
+    <t>6788161235286</t>
+  </si>
+  <si>
+    <t>dosen117</t>
+  </si>
+  <si>
+    <t>Dosen 117</t>
+  </si>
+  <si>
+    <t>dosen117@example.com</t>
+  </si>
+  <si>
+    <t>8846266771321</t>
+  </si>
+  <si>
+    <t>dosen118</t>
+  </si>
+  <si>
+    <t>Dosen 118</t>
+  </si>
+  <si>
+    <t>dosen118@example.com</t>
+  </si>
+  <si>
+    <t>4544886229633</t>
+  </si>
+  <si>
+    <t>dosen119</t>
+  </si>
+  <si>
+    <t>Dosen 119</t>
+  </si>
+  <si>
+    <t>dosen119@example.com</t>
+  </si>
+  <si>
+    <t>8787825954589</t>
+  </si>
+  <si>
+    <t>dosen120</t>
+  </si>
+  <si>
+    <t>Dosen 120</t>
+  </si>
+  <si>
+    <t>dosen120@example.com</t>
+  </si>
+  <si>
+    <t>5843817115897</t>
+  </si>
+  <si>
+    <t>dosen121</t>
+  </si>
+  <si>
+    <t>Dosen 121</t>
+  </si>
+  <si>
+    <t>dosen121@example.com</t>
+  </si>
+  <si>
+    <t>7578940484450</t>
+  </si>
+  <si>
+    <t>dosen122</t>
+  </si>
+  <si>
+    <t>Dosen 122</t>
+  </si>
+  <si>
+    <t>dosen122@example.com</t>
+  </si>
+  <si>
+    <t>2876632559594</t>
+  </si>
+  <si>
+    <t>dosen123</t>
+  </si>
+  <si>
+    <t>Dosen 123</t>
+  </si>
+  <si>
+    <t>dosen123@example.com</t>
+  </si>
+  <si>
+    <t>1713183212824</t>
+  </si>
+  <si>
+    <t>dosen124</t>
+  </si>
+  <si>
+    <t>Dosen 124</t>
+  </si>
+  <si>
+    <t>dosen124@example.com</t>
+  </si>
+  <si>
+    <t>9461328236178</t>
+  </si>
+  <si>
+    <t>dosen125</t>
+  </si>
+  <si>
+    <t>Dosen 125</t>
+  </si>
+  <si>
+    <t>dosen125@example.com</t>
+  </si>
+  <si>
+    <t>6835220508593</t>
+  </si>
+  <si>
+    <t>dosen126</t>
+  </si>
+  <si>
+    <t>Dosen 126</t>
+  </si>
+  <si>
+    <t>dosen126@example.com</t>
+  </si>
+  <si>
+    <t>9576474300859</t>
+  </si>
+  <si>
+    <t>dosen127</t>
+  </si>
+  <si>
+    <t>Dosen 127</t>
+  </si>
+  <si>
+    <t>dosen127@example.com</t>
+  </si>
+  <si>
+    <t>2536964693493</t>
+  </si>
+  <si>
+    <t>dosen128</t>
+  </si>
+  <si>
+    <t>Dosen 128</t>
+  </si>
+  <si>
+    <t>dosen128@example.com</t>
+  </si>
+  <si>
+    <t>9229635549820</t>
+  </si>
+  <si>
+    <t>dosen129</t>
+  </si>
+  <si>
+    <t>Dosen 129</t>
+  </si>
+  <si>
+    <t>dosen129@example.com</t>
+  </si>
+  <si>
+    <t>8229912990760</t>
+  </si>
+  <si>
+    <t>dosen130</t>
+  </si>
+  <si>
+    <t>Dosen 130</t>
+  </si>
+  <si>
+    <t>dosen130@example.com</t>
+  </si>
+  <si>
+    <t>8131095060661</t>
+  </si>
+  <si>
+    <t>dosen131</t>
+  </si>
+  <si>
+    <t>Dosen 131</t>
+  </si>
+  <si>
+    <t>dosen131@example.com</t>
+  </si>
+  <si>
+    <t>4997568490214</t>
+  </si>
+  <si>
+    <t>dosen132</t>
+  </si>
+  <si>
+    <t>Dosen 132</t>
+  </si>
+  <si>
+    <t>dosen132@example.com</t>
+  </si>
+  <si>
+    <t>9047280081692</t>
+  </si>
+  <si>
+    <t>dosen133</t>
+  </si>
+  <si>
+    <t>Dosen 133</t>
+  </si>
+  <si>
+    <t>dosen133@example.com</t>
+  </si>
+  <si>
+    <t>3707864925528</t>
+  </si>
+  <si>
+    <t>dosen134</t>
+  </si>
+  <si>
+    <t>Dosen 134</t>
+  </si>
+  <si>
+    <t>dosen134@example.com</t>
+  </si>
+  <si>
+    <t>8171681179091</t>
+  </si>
+  <si>
+    <t>dosen135</t>
+  </si>
+  <si>
+    <t>Dosen 135</t>
+  </si>
+  <si>
+    <t>dosen135@example.com</t>
+  </si>
+  <si>
+    <t>6195911563410</t>
+  </si>
+  <si>
+    <t>dosen136</t>
+  </si>
+  <si>
+    <t>Dosen 136</t>
+  </si>
+  <si>
+    <t>dosen136@example.com</t>
+  </si>
+  <si>
+    <t>3785084993120</t>
+  </si>
+  <si>
+    <t>dosen137</t>
+  </si>
+  <si>
+    <t>Dosen 137</t>
+  </si>
+  <si>
+    <t>dosen137@example.com</t>
+  </si>
+  <si>
+    <t>5428818545643</t>
+  </si>
+  <si>
+    <t>dosen138</t>
+  </si>
+  <si>
+    <t>Dosen 138</t>
+  </si>
+  <si>
+    <t>dosen138@example.com</t>
+  </si>
+  <si>
+    <t>8911451290867</t>
+  </si>
+  <si>
+    <t>dosen139</t>
+  </si>
+  <si>
+    <t>Dosen 139</t>
+  </si>
+  <si>
+    <t>dosen139@example.com</t>
+  </si>
+  <si>
+    <t>4666858915626</t>
+  </si>
+  <si>
+    <t>dosen140</t>
+  </si>
+  <si>
+    <t>Dosen 140</t>
+  </si>
+  <si>
+    <t>dosen140@example.com</t>
+  </si>
+  <si>
+    <t>6385145052452</t>
+  </si>
+  <si>
+    <t>dosen141</t>
+  </si>
+  <si>
+    <t>Dosen 141</t>
+  </si>
+  <si>
+    <t>dosen141@example.com</t>
+  </si>
+  <si>
+    <t>3254167854735</t>
+  </si>
+  <si>
+    <t>dosen142</t>
+  </si>
+  <si>
+    <t>Dosen 142</t>
+  </si>
+  <si>
+    <t>dosen142@example.com</t>
+  </si>
+  <si>
+    <t>5442794997075</t>
+  </si>
+  <si>
+    <t>dosen143</t>
+  </si>
+  <si>
+    <t>Dosen 143</t>
+  </si>
+  <si>
+    <t>dosen143@example.com</t>
+  </si>
+  <si>
+    <t>3241411140626</t>
+  </si>
+  <si>
+    <t>dosen144</t>
+  </si>
+  <si>
+    <t>Dosen 144</t>
+  </si>
+  <si>
+    <t>dosen144@example.com</t>
+  </si>
+  <si>
+    <t>7962048296364</t>
+  </si>
+  <si>
+    <t>dosen145</t>
+  </si>
+  <si>
+    <t>Dosen 145</t>
+  </si>
+  <si>
+    <t>dosen145@example.com</t>
+  </si>
+  <si>
+    <t>1147824499108</t>
+  </si>
+  <si>
+    <t>dosen146</t>
+  </si>
+  <si>
+    <t>Dosen 146</t>
+  </si>
+  <si>
+    <t>dosen146@example.com</t>
+  </si>
+  <si>
+    <t>2936431633990</t>
+  </si>
+  <si>
+    <t>dosen147</t>
+  </si>
+  <si>
+    <t>Dosen 147</t>
+  </si>
+  <si>
+    <t>dosen147@example.com</t>
+  </si>
+  <si>
+    <t>3695471519956</t>
+  </si>
+  <si>
+    <t>dosen148</t>
+  </si>
+  <si>
+    <t>Dosen 148</t>
+  </si>
+  <si>
+    <t>dosen148@example.com</t>
+  </si>
+  <si>
+    <t>2388235338957</t>
+  </si>
+  <si>
+    <t>dosen149</t>
+  </si>
+  <si>
+    <t>Dosen 149</t>
+  </si>
+  <si>
+    <t>dosen149@example.com</t>
+  </si>
+  <si>
+    <t>2053720969926</t>
+  </si>
+  <si>
+    <t>dosen150</t>
+  </si>
+  <si>
+    <t>Dosen 150</t>
+  </si>
+  <si>
+    <t>dosen150@example.com</t>
+  </si>
+  <si>
+    <t>5124405682444</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,14 +679,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,17 +701,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1809E43-865B-409B-A77C-B67138C2CBDC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,26 +1055,873 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>12345</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>987654321</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{372330C7-CCF4-40B8-B924-39190DC0F96C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>